<commit_message>
added visual report image
</commit_message>
<xml_diff>
--- a/Jaidi_report.xlsx
+++ b/Jaidi_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S537520\Desktop\spark-wordcount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CB8410F6-EB17-4B58-8EC6-17C9BED74ADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5391DD32-3729-42FA-98DA-6DA0D29311B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
@@ -5119,16 +5119,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>305026</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>63262</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>306159</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>301385</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>174267</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5455,11 +5455,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>